<commit_message>
Fixes total coal values in historical extension
</commit_message>
<xml_diff>
--- a/input/mappings/Bond/Bond_sector_ext_map.xlsx
+++ b/input/mappings/Bond/Bond_sector_ext_map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="360" windowWidth="11200" windowHeight="12680" tabRatio="500"/>
+    <workbookView xWindow="7620" yWindow="360" windowWidth="11200" windowHeight="12680" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bond_to_ext" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
   <si>
     <t>Tech</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>RCO</t>
+  </si>
+  <si>
+    <t>Power</t>
   </si>
 </sst>
 </file>
@@ -668,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -891,7 +894,7 @@
         <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -963,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -985,7 +988,7 @@
         <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -993,7 +996,7 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1001,7 +1004,7 @@
         <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2">

</xml_diff>

<commit_message>
CEDS Data and exogenous assumptions updates
</commit_message>
<xml_diff>
--- a/input/mappings/Bond/Bond_sector_ext_map.xlsx
+++ b/input/mappings/Bond/Bond_sector_ext_map.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoes919/Documents/CEDS/input/mappings/Bond/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="360" windowWidth="30100" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="1260" yWindow="820" windowWidth="30100" windowHeight="18380" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bond_to_ext" sheetId="1" r:id="rId1"/>
     <sheet name="CEDS_to_ext" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
   <si>
     <t>Tech</t>
   </si>
@@ -230,12 +235,27 @@
   </si>
   <si>
     <t>1A3dii_Domestic-navigation</t>
+  </si>
+  <si>
+    <t>Other_tranformation</t>
+  </si>
+  <si>
+    <t>1A1bc_Other-transformation</t>
+  </si>
+  <si>
+    <t>Other_transformation</t>
+  </si>
+  <si>
+    <t>1A1bc_Other-feedstocks</t>
+  </si>
+  <si>
+    <t>Other_feedstocks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -344,6 +364,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -668,16 +696,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -688,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -699,7 +730,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -710,7 +741,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -721,7 +752,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -732,7 +763,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -743,7 +774,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -754,7 +785,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -765,7 +796,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -776,7 +807,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -784,7 +815,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -792,7 +823,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -800,7 +831,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -808,7 +839,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -816,7 +847,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -827,7 +858,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -838,7 +869,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -846,7 +877,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -854,7 +885,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -862,7 +893,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -870,7 +901,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -878,7 +909,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -886,7 +917,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -897,7 +928,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -905,7 +936,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -913,7 +944,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -924,23 +955,29 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>40</v>
       </c>
       <c r="B27" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="C27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>41</v>
       </c>
       <c r="B28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="C28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -963,19 +1000,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -983,7 +1020,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -991,7 +1028,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -999,7 +1036,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -1007,7 +1044,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -1015,7 +1052,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -1023,7 +1060,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -1031,7 +1068,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
@@ -1039,7 +1076,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -1047,7 +1084,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -1055,7 +1092,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -1063,7 +1100,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
@@ -1071,7 +1108,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
@@ -1079,7 +1116,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -1087,7 +1124,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>59</v>
       </c>
@@ -1095,7 +1132,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>60</v>
       </c>
@@ -1103,7 +1140,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>61</v>
       </c>
@@ -1111,7 +1148,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
@@ -1119,7 +1156,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>63</v>
       </c>
@@ -1127,7 +1164,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1135,7 +1172,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>15</v>
       </c>
@@ -1143,7 +1180,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1151,7 +1188,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -1159,7 +1196,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
@@ -1167,7 +1204,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
@@ -1175,7 +1212,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1183,7 +1220,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>43</v>
       </c>
@@ -1191,12 +1228,28 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Public full release (#19)
* Fixes to user-defined energy data
* Fix_metadata_collate
* Rename processing scripts
* Modify input and output directories for user-defined energy scripts
* Add option to clean user-defined-energy to Makefile
* Modify Makefile to clean additional diagnostic directories
* Move log directory to top-level
* Remove duplicate and/or unused files
* Correct shipping fuel time series.
* Correct UN energy data negative values
* Update waste emissions code and assumptions
* Update korea bcoc
* Update README for release
</commit_message>
<xml_diff>
--- a/input/mappings/Bond/Bond_sector_ext_map.xlsx
+++ b/input/mappings/Bond/Bond_sector_ext_map.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orou913\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orou913\Desktop\CEDS-Repositories\CEDS_mass_balance\CEDS\input\mappings\Bond\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580FE038-7B3B-42C1-A500-AFFB7F8F2B86}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="825" windowWidth="30105" windowHeight="18375" tabRatio="500"/>
+    <workbookView xWindow="2685" yWindow="1290" windowWidth="23415" windowHeight="14190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bond_to_ext" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="75">
   <si>
     <t>Tech</t>
   </si>
@@ -255,7 +256,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -696,11 +697,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1000,11 +1001,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1184,9 +1185,6 @@
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B22" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">

</xml_diff>